<commit_message>
Refactor done. Using class Case now
Unfortunately, and surpisingly, no performance win. Before refactor 10000
lines in 21 sec. After refactor in 25 sec. But definitely a big win in
readability
</commit_message>
<xml_diff>
--- a/input.example.xlsx
+++ b/input.example.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abos\Documents\Python\generate-process-mining-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2283DD1-47FF-4137-803E-7EF6A9FEE598}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FECA83-7A69-4D43-8848-57D0DEC8AE38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{D7EB7520-79AA-48AA-A273-C669DE671554}"/>
   </bookViews>
   <sheets>
-    <sheet name="activity" sheetId="1" r:id="rId1"/>
+    <sheet name="step" sheetId="1" r:id="rId1"/>
     <sheet name="process_flow" sheetId="2" r:id="rId2"/>
     <sheet name="case_property" sheetId="3" r:id="rId3"/>
-    <sheet name="activity_property" sheetId="4" r:id="rId4"/>
+    <sheet name="step_property" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>duration</t>
   </si>
@@ -62,18 +62,6 @@
     <t>property_type</t>
   </si>
   <si>
-    <t>activity_id</t>
-  </si>
-  <si>
-    <t>activity_name</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>next_activity_id</t>
-  </si>
-  <si>
     <t>Medewerker</t>
   </si>
   <si>
@@ -102,6 +90,21 @@
   </si>
   <si>
     <t>outliers</t>
+  </si>
+  <si>
+    <t>Traject</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>step_id</t>
+  </si>
+  <si>
+    <t>step_name</t>
+  </si>
+  <si>
+    <t>next_step_id</t>
   </si>
 </sst>
 </file>
@@ -487,7 +490,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,21 +500,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>0</v>
+      <c r="A2" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -525,7 +528,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -674,7 +677,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,18 +687,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -705,8 +708,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -797,7 +800,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -830,7 +833,7 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -872,10 +875,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>0.6</v>
@@ -883,10 +886,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>0.4</v>
@@ -894,10 +897,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>0.1</v>
@@ -905,10 +908,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>0.2</v>
@@ -916,10 +919,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>0.3</v>
@@ -927,10 +930,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
       </c>
       <c r="C7">
         <v>0.4</v>
@@ -943,7 +946,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CE1B20-46E6-4980-A8AF-9F6BC4A06476}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -956,7 +959,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
@@ -973,7 +976,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -987,7 +990,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1001,7 +1004,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1010,7 +1013,36 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>0.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implement waiting time after step
Its working. But still using global df_step in the Case methods is not so neat
</commit_message>
<xml_diff>
--- a/input.example.xlsx
+++ b/input.example.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abos\Documents\Python\generate-process-mining-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FECA83-7A69-4D43-8848-57D0DEC8AE38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DBA11B-BA5C-421E-8E96-D8CDBF4CB959}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{D7EB7520-79AA-48AA-A273-C669DE671554}"/>
   </bookViews>
   <sheets>
     <sheet name="step" sheetId="1" r:id="rId1"/>
     <sheet name="process_flow" sheetId="2" r:id="rId2"/>
-    <sheet name="case_property" sheetId="3" r:id="rId3"/>
-    <sheet name="step_property" sheetId="4" r:id="rId4"/>
+    <sheet name="case_property (todo)" sheetId="3" r:id="rId3"/>
+    <sheet name="step_property (todo)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>duration</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>next_step_id</t>
+  </si>
+  <si>
+    <t>wait_time</t>
   </si>
 </sst>
 </file>
@@ -487,18 +490,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B00464-A0A5-411E-8E7D-92E8B599BA94}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
+    <col min="1" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -511,8 +514,11 @@
       <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -525,8 +531,11 @@
       <c r="D2" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -539,8 +548,11 @@
       <c r="D3" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -553,8 +565,11 @@
       <c r="D4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -565,10 +580,13 @@
         <v>10</v>
       </c>
       <c r="D5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -576,13 +594,16 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -595,8 +616,11 @@
       <c r="D7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -609,8 +633,11 @@
       <c r="D8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -621,10 +648,13 @@
         <v>20</v>
       </c>
       <c r="D9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -637,8 +667,11 @@
       <c r="D10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -651,8 +684,11 @@
       <c r="D11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -663,6 +699,9 @@
         <v>50</v>
       </c>
       <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement case properties (Excel, code and output)
</commit_message>
<xml_diff>
--- a/input.example.xlsx
+++ b/input.example.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abos\Documents\Python\generate-process-mining-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DBA11B-BA5C-421E-8E96-D8CDBF4CB959}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219EF18C-9245-496D-88F0-96348CAD86DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{D7EB7520-79AA-48AA-A273-C669DE671554}"/>
   </bookViews>
   <sheets>
-    <sheet name="step" sheetId="1" r:id="rId1"/>
+    <sheet name="steps" sheetId="1" r:id="rId1"/>
     <sheet name="process_flow" sheetId="2" r:id="rId2"/>
-    <sheet name="case_property (todo)" sheetId="3" r:id="rId3"/>
-    <sheet name="step_property (todo)" sheetId="4" r:id="rId4"/>
+    <sheet name="case_properties" sheetId="3" r:id="rId3"/>
+    <sheet name="step_properties (todo)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,9 +56,6 @@
     <t>Interim medewerker</t>
   </si>
   <si>
-    <t>property</t>
-  </si>
-  <si>
     <t>property_type</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>outliers</t>
-  </si>
-  <si>
     <t>Traject</t>
   </si>
   <si>
@@ -108,6 +102,12 @@
   </si>
   <si>
     <t>wait_time</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>has_outliers</t>
   </si>
 </sst>
 </file>
@@ -492,9 +492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B00464-A0A5-411E-8E7D-92E8B599BA94}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -503,19 +501,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -716,7 +714,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A8" sqref="A8:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,10 +724,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -892,9 +890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7293AFC2-F934-4038-BF39-965256578273}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -903,10 +899,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -914,10 +910,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
       </c>
       <c r="C2">
         <v>0.6</v>
@@ -925,10 +921,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>0.4</v>
@@ -936,10 +932,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
       </c>
       <c r="C4">
         <v>0.1</v>
@@ -947,10 +943,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>0.2</v>
@@ -958,10 +954,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>0.3</v>
@@ -969,10 +965,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>0.4</v>
@@ -987,9 +983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CE1B20-46E6-4980-A8AF-9F6BC4A06476}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -998,13 +992,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1015,7 +1009,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1029,7 +1023,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1043,7 +1037,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1057,10 +1051,10 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>0.3</v>
@@ -1071,10 +1065,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>0.7</v>

</xml_diff>